<commit_message>
Update reports and data quality checks
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_senegal.xlsx
+++ b/inst/extdata/main_dict_senegal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="602">
   <si>
     <t>old</t>
   </si>
@@ -1532,9 +1532,6 @@
     <t>a4_c_9</t>
   </si>
   <si>
-    <t>crfs-t02b-a4_c_4</t>
-  </si>
-  <si>
     <t>a4_c_4</t>
   </si>
   <si>
@@ -1824,6 +1821,15 @@
   </si>
   <si>
     <t>crfs-t07a-tt06a-d2_3b</t>
+  </si>
+  <si>
+    <t>crfs-t02b-location_name</t>
+  </si>
+  <si>
+    <t>crfs-t02b-a4_c_6</t>
+  </si>
+  <si>
+    <t>cg_district</t>
   </si>
 </sst>
 </file>
@@ -2244,10 +2250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H203"/>
+  <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="D184" sqref="D184"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2281,7 +2287,7 @@
         <v>172</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>194</v>
@@ -3043,37 +3049,37 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>509</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="12" t="s">
         <v>510</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="4">
-        <v>1</v>
-      </c>
-      <c r="F31" s="3">
-        <v>1</v>
-      </c>
-      <c r="G31" s="3">
-        <v>1</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
+        <v>512</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>513</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>514</v>
-      </c>
       <c r="C32" s="2">
         <v>1</v>
       </c>
@@ -3090,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -3745,11 +3751,11 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="B58" s="19" t="s">
         <v>505</v>
       </c>
-      <c r="B58" s="19" t="s">
-        <v>506</v>
-      </c>
       <c r="C58" s="2">
         <v>1</v>
       </c>
@@ -3766,16 +3772,16 @@
         <v>1</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>507</v>
       </c>
-      <c r="B59" s="19" t="s">
-        <v>508</v>
-      </c>
       <c r="C59" s="2">
         <v>1</v>
       </c>
@@ -3792,75 +3798,75 @@
         <v>1</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4">
+        <v>1</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <v>1</v>
+      </c>
+      <c r="H60" s="11" t="s">
         <v>502</v>
       </c>
-      <c r="B60" s="11" t="s">
-        <v>504</v>
-      </c>
-      <c r="C60" s="2">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2">
-        <v>1</v>
-      </c>
-      <c r="E60" s="4">
-        <v>1</v>
-      </c>
-      <c r="F60" s="4">
-        <v>0</v>
-      </c>
-      <c r="G60" s="3">
-        <v>1</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>503</v>
-      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>52</v>
+      <c r="A61" s="11" t="s">
+        <v>600</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>601</v>
       </c>
       <c r="C61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" s="4">
         <v>1</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="4">
         <v>0</v>
       </c>
       <c r="G61" s="3">
         <v>1</v>
       </c>
-      <c r="H61" s="13" t="s">
-        <v>218</v>
+      <c r="H61" s="11" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C62" s="20">
-        <v>0</v>
-      </c>
-      <c r="D62" s="20">
-        <v>0</v>
-      </c>
-      <c r="E62" s="21">
+        <v>52</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="4">
         <v>1</v>
       </c>
       <c r="F62" s="3">
@@ -3870,15 +3876,15 @@
         <v>1</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C63" s="20">
         <v>0</v>
@@ -3886,7 +3892,7 @@
       <c r="D63" s="20">
         <v>0</v>
       </c>
-      <c r="E63" s="20">
+      <c r="E63" s="21">
         <v>1</v>
       </c>
       <c r="F63" s="3">
@@ -3896,15 +3902,15 @@
         <v>1</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C64" s="20">
         <v>0</v>
@@ -3912,7 +3918,7 @@
       <c r="D64" s="20">
         <v>0</v>
       </c>
-      <c r="E64" s="21">
+      <c r="E64" s="20">
         <v>1</v>
       </c>
       <c r="F64" s="3">
@@ -3922,15 +3928,15 @@
         <v>1</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C65" s="20">
         <v>0</v>
@@ -3948,23 +3954,23 @@
         <v>1</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C66" s="2">
-        <v>0</v>
-      </c>
-      <c r="D66" s="2">
-        <v>0</v>
-      </c>
-      <c r="E66" s="4">
+        <v>56</v>
+      </c>
+      <c r="C66" s="20">
+        <v>0</v>
+      </c>
+      <c r="D66" s="20">
+        <v>0</v>
+      </c>
+      <c r="E66" s="21">
         <v>1</v>
       </c>
       <c r="F66" s="3">
@@ -3974,15 +3980,15 @@
         <v>1</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C67" s="2">
         <v>0</v>
@@ -4000,15 +4006,15 @@
         <v>1</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C68" s="2">
         <v>0</v>
@@ -4026,15 +4032,15 @@
         <v>1</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
@@ -4052,15 +4058,15 @@
         <v>1</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C70" s="2">
         <v>0</v>
@@ -4078,15 +4084,15 @@
         <v>1</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C71" s="2">
         <v>0</v>
@@ -4104,15 +4110,15 @@
         <v>1</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C72" s="2">
         <v>0</v>
@@ -4130,15 +4136,15 @@
         <v>1</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73" s="2">
         <v>0</v>
@@ -4156,15 +4162,15 @@
         <v>1</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C74" s="2">
         <v>0</v>
@@ -4182,15 +4188,15 @@
         <v>1</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -4208,15 +4214,15 @@
         <v>1</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
@@ -4234,15 +4240,15 @@
         <v>1</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C77" s="2">
         <v>0</v>
@@ -4260,15 +4266,15 @@
         <v>1</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C78" s="2">
         <v>0</v>
@@ -4286,15 +4292,15 @@
         <v>1</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C79" s="2">
         <v>0</v>
@@ -4312,15 +4318,15 @@
         <v>1</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C80" s="2">
         <v>0</v>
@@ -4338,23 +4344,23 @@
         <v>1</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C81" s="20">
+        <v>71</v>
+      </c>
+      <c r="C81" s="2">
         <v>0</v>
       </c>
       <c r="D81" s="2">
         <v>0</v>
       </c>
-      <c r="E81" s="21">
+      <c r="E81" s="4">
         <v>1</v>
       </c>
       <c r="F81" s="3">
@@ -4364,15 +4370,15 @@
         <v>1</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C82" s="20">
         <v>0</v>
@@ -4380,7 +4386,7 @@
       <c r="D82" s="2">
         <v>0</v>
       </c>
-      <c r="E82" s="20">
+      <c r="E82" s="21">
         <v>1</v>
       </c>
       <c r="F82" s="3">
@@ -4390,15 +4396,15 @@
         <v>1</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C83" s="20">
         <v>0</v>
@@ -4406,7 +4412,7 @@
       <c r="D83" s="2">
         <v>0</v>
       </c>
-      <c r="E83" s="21">
+      <c r="E83" s="20">
         <v>1</v>
       </c>
       <c r="F83" s="3">
@@ -4416,15 +4422,15 @@
         <v>1</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C84" s="20">
         <v>0</v>
@@ -4442,15 +4448,15 @@
         <v>1</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C85" s="20">
         <v>0</v>
@@ -4458,7 +4464,7 @@
       <c r="D85" s="2">
         <v>0</v>
       </c>
-      <c r="E85" s="20">
+      <c r="E85" s="21">
         <v>1</v>
       </c>
       <c r="F85" s="3">
@@ -4468,15 +4474,15 @@
         <v>1</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C86" s="20">
         <v>0</v>
@@ -4484,7 +4490,7 @@
       <c r="D86" s="2">
         <v>0</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E86" s="20">
         <v>1</v>
       </c>
       <c r="F86" s="3">
@@ -4494,15 +4500,15 @@
         <v>1</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C87" s="20">
         <v>0</v>
@@ -4520,17 +4526,17 @@
         <v>1</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C88" s="2">
+        <v>78</v>
+      </c>
+      <c r="C88" s="20">
         <v>0</v>
       </c>
       <c r="D88" s="2">
@@ -4546,67 +4552,67 @@
         <v>1</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0</v>
+      </c>
+      <c r="E89" s="4">
+        <v>1</v>
+      </c>
+      <c r="F89" s="3">
+        <v>0</v>
+      </c>
+      <c r="G89" s="3">
+        <v>1</v>
+      </c>
+      <c r="H89" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B90" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C89" s="2">
-        <v>0</v>
-      </c>
-      <c r="D89" s="2">
-        <v>0</v>
-      </c>
-      <c r="E89" s="4">
-        <v>1</v>
-      </c>
-      <c r="F89" s="3">
-        <v>0</v>
-      </c>
-      <c r="G89" s="3">
-        <v>1</v>
-      </c>
-      <c r="H89" s="13" t="s">
+      <c r="C90" s="2">
+        <v>0</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0</v>
+      </c>
+      <c r="E90" s="4">
+        <v>1</v>
+      </c>
+      <c r="F90" s="3">
+        <v>0</v>
+      </c>
+      <c r="G90" s="3">
+        <v>1</v>
+      </c>
+      <c r="H90" s="13" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="17" t="s">
-        <v>408</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90" s="2">
-        <v>0</v>
-      </c>
-      <c r="D90" s="2">
-        <v>0</v>
-      </c>
-      <c r="E90" s="2">
-        <v>1</v>
-      </c>
-      <c r="F90" s="3">
-        <v>1</v>
-      </c>
-      <c r="G90" s="3">
-        <v>1</v>
-      </c>
-      <c r="H90" s="17" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C91" s="2">
         <v>0</v>
@@ -4621,18 +4627,18 @@
         <v>1</v>
       </c>
       <c r="G91" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C92" s="2">
         <v>0</v>
@@ -4650,15 +4656,15 @@
         <v>0</v>
       </c>
       <c r="H92" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C93" s="2">
         <v>0</v>
@@ -4676,15 +4682,15 @@
         <v>0</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C94" s="2">
         <v>0</v>
@@ -4702,15 +4708,15 @@
         <v>0</v>
       </c>
       <c r="H94" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C95" s="2">
         <v>0</v>
@@ -4728,15 +4734,15 @@
         <v>0</v>
       </c>
       <c r="H95" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C96" s="2">
         <v>0</v>
@@ -4754,15 +4760,15 @@
         <v>0</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C97" s="2">
         <v>0</v>
@@ -4780,15 +4786,15 @@
         <v>0</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C98" s="2">
         <v>0</v>
@@ -4806,15 +4812,15 @@
         <v>0</v>
       </c>
       <c r="H98" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C99" s="2">
         <v>0</v>
@@ -4832,15 +4838,15 @@
         <v>0</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C100" s="2">
         <v>0</v>
@@ -4858,15 +4864,15 @@
         <v>0</v>
       </c>
       <c r="H100" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
@@ -4884,15 +4890,15 @@
         <v>0</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C102" s="2">
         <v>0</v>
@@ -4910,15 +4916,15 @@
         <v>0</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
@@ -4936,15 +4942,15 @@
         <v>0</v>
       </c>
       <c r="H103" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
@@ -4962,15 +4968,15 @@
         <v>0</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C105" s="2">
         <v>0</v>
@@ -4988,15 +4994,15 @@
         <v>0</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
@@ -5014,15 +5020,15 @@
         <v>0</v>
       </c>
       <c r="H106" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C107" s="2">
         <v>0</v>
@@ -5037,18 +5043,18 @@
         <v>1</v>
       </c>
       <c r="G107" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>427</v>
-      </c>
-      <c r="B108" s="15" t="s">
-        <v>99</v>
+        <v>426</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>98</v>
       </c>
       <c r="C108" s="2">
         <v>0</v>
@@ -5066,15 +5072,15 @@
         <v>1</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
@@ -5092,15 +5098,15 @@
         <v>1</v>
       </c>
       <c r="H109" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C110" s="2">
         <v>0</v>
@@ -5118,15 +5124,15 @@
         <v>1</v>
       </c>
       <c r="H110" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
@@ -5144,15 +5150,15 @@
         <v>1</v>
       </c>
       <c r="H111" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C112" s="2">
         <v>0</v>
@@ -5170,15 +5176,15 @@
         <v>1</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C113" s="2">
         <v>0</v>
@@ -5196,15 +5202,15 @@
         <v>1</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C114" s="2">
         <v>0</v>
@@ -5222,15 +5228,15 @@
         <v>1</v>
       </c>
       <c r="H114" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C115" s="2">
         <v>0</v>
@@ -5238,25 +5244,25 @@
       <c r="D115" s="2">
         <v>0</v>
       </c>
-      <c r="E115" s="20">
-        <v>1</v>
-      </c>
-      <c r="F115" s="22">
+      <c r="E115" s="2">
+        <v>1</v>
+      </c>
+      <c r="F115" s="3">
         <v>1</v>
       </c>
       <c r="G115" s="3">
         <v>1</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C116" s="2">
         <v>0</v>
@@ -5274,15 +5280,15 @@
         <v>1</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C117" s="2">
         <v>0</v>
@@ -5300,15 +5306,15 @@
         <v>1</v>
       </c>
       <c r="H117" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C118" s="2">
         <v>0</v>
@@ -5319,22 +5325,22 @@
       <c r="E118" s="20">
         <v>1</v>
       </c>
-      <c r="F118" s="20">
+      <c r="F118" s="22">
         <v>1</v>
       </c>
       <c r="G118" s="3">
         <v>1</v>
       </c>
       <c r="H118" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C119" s="2">
         <v>0</v>
@@ -5345,22 +5351,22 @@
       <c r="E119" s="20">
         <v>1</v>
       </c>
-      <c r="F119" s="22">
+      <c r="F119" s="20">
         <v>1</v>
       </c>
       <c r="G119" s="3">
         <v>1</v>
       </c>
       <c r="H119" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C120" s="2">
         <v>0</v>
@@ -5378,15 +5384,15 @@
         <v>1</v>
       </c>
       <c r="H120" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C121" s="2">
         <v>0</v>
@@ -5404,15 +5410,15 @@
         <v>1</v>
       </c>
       <c r="H121" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C122" s="2">
         <v>0</v>
@@ -5423,22 +5429,22 @@
       <c r="E122" s="20">
         <v>1</v>
       </c>
-      <c r="F122" s="20">
+      <c r="F122" s="22">
         <v>1</v>
       </c>
       <c r="G122" s="3">
         <v>1</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
-        <v>442</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>114</v>
+        <v>441</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="C123" s="2">
         <v>0</v>
@@ -5449,22 +5455,22 @@
       <c r="E123" s="20">
         <v>1</v>
       </c>
-      <c r="F123" s="22">
+      <c r="F123" s="20">
         <v>1</v>
       </c>
       <c r="G123" s="3">
         <v>1</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C124" s="2">
         <v>0</v>
@@ -5479,18 +5485,18 @@
         <v>1</v>
       </c>
       <c r="G124" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>115</v>
+        <v>280</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C125" s="2">
         <v>0</v>
@@ -5508,15 +5514,15 @@
         <v>0</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>281</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C126" s="2">
         <v>0</v>
@@ -5534,15 +5540,15 @@
         <v>0</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C127" s="2">
         <v>0</v>
@@ -5560,15 +5566,15 @@
         <v>0</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C128" s="2">
         <v>0</v>
@@ -5579,22 +5585,22 @@
       <c r="E128" s="20">
         <v>1</v>
       </c>
-      <c r="F128" s="20">
+      <c r="F128" s="22">
         <v>1</v>
       </c>
       <c r="G128" s="3">
         <v>0</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C129" s="2">
         <v>0</v>
@@ -5605,22 +5611,22 @@
       <c r="E129" s="20">
         <v>1</v>
       </c>
-      <c r="F129" s="22">
+      <c r="F129" s="20">
         <v>1</v>
       </c>
       <c r="G129" s="3">
         <v>0</v>
       </c>
       <c r="H129" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C130" s="2">
         <v>0</v>
@@ -5638,67 +5644,67 @@
         <v>0</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C131" s="2">
+        <v>0</v>
+      </c>
+      <c r="D131" s="2">
+        <v>0</v>
+      </c>
+      <c r="E131" s="20">
+        <v>1</v>
+      </c>
+      <c r="F131" s="22">
+        <v>1</v>
+      </c>
+      <c r="G131" s="3">
+        <v>0</v>
+      </c>
+      <c r="H131" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" s="17" t="s">
         <v>450</v>
       </c>
-      <c r="B131" s="14" t="s">
+      <c r="B132" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C131" s="2">
-        <v>0</v>
-      </c>
-      <c r="D131" s="2">
-        <v>0</v>
-      </c>
-      <c r="E131" s="20">
-        <v>1</v>
-      </c>
-      <c r="F131" s="22">
-        <v>1</v>
-      </c>
-      <c r="G131" s="3">
-        <v>0</v>
-      </c>
-      <c r="H131" s="17" t="s">
+      <c r="C132" s="2">
+        <v>0</v>
+      </c>
+      <c r="D132" s="2">
+        <v>0</v>
+      </c>
+      <c r="E132" s="20">
+        <v>1</v>
+      </c>
+      <c r="F132" s="22">
+        <v>1</v>
+      </c>
+      <c r="G132" s="3">
+        <v>0</v>
+      </c>
+      <c r="H132" s="17" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="18" t="s">
-        <v>576</v>
-      </c>
-      <c r="B132" s="16" t="s">
-        <v>582</v>
-      </c>
-      <c r="C132" s="2">
-        <v>0</v>
-      </c>
-      <c r="D132" s="2">
-        <v>0</v>
-      </c>
-      <c r="E132" s="20">
-        <v>1</v>
-      </c>
-      <c r="F132" s="20">
-        <v>1</v>
-      </c>
-      <c r="G132" s="3">
-        <v>0</v>
-      </c>
-      <c r="H132" s="18" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="18" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C133" s="2">
         <v>0</v>
@@ -5716,15 +5722,15 @@
         <v>0</v>
       </c>
       <c r="H133" s="18" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="18" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C134" s="2">
         <v>0</v>
@@ -5742,15 +5748,15 @@
         <v>0</v>
       </c>
       <c r="H134" s="18" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="18" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C135" s="2">
         <v>0</v>
@@ -5768,15 +5774,15 @@
         <v>0</v>
       </c>
       <c r="H135" s="18" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="18" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C136" s="2">
         <v>0</v>
@@ -5794,15 +5800,15 @@
         <v>0</v>
       </c>
       <c r="H136" s="18" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="18" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C137" s="2">
         <v>0</v>
@@ -5820,15 +5826,15 @@
         <v>0</v>
       </c>
       <c r="H137" s="18" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="17" t="s">
-        <v>451</v>
-      </c>
-      <c r="B138" s="14" t="s">
-        <v>123</v>
+      <c r="A138" s="18" t="s">
+        <v>580</v>
+      </c>
+      <c r="B138" s="16" t="s">
+        <v>586</v>
       </c>
       <c r="C138" s="2">
         <v>0</v>
@@ -5839,22 +5845,22 @@
       <c r="E138" s="20">
         <v>1</v>
       </c>
-      <c r="F138" s="22">
+      <c r="F138" s="20">
         <v>1</v>
       </c>
       <c r="G138" s="3">
         <v>0</v>
       </c>
-      <c r="H138" s="17" t="s">
-        <v>288</v>
+      <c r="H138" s="18" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="17" t="s">
-        <v>558</v>
-      </c>
-      <c r="B139" s="23" t="s">
-        <v>534</v>
+        <v>451</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="C139" s="2">
         <v>0</v>
@@ -5862,7 +5868,7 @@
       <c r="D139" s="2">
         <v>0</v>
       </c>
-      <c r="E139" s="4">
+      <c r="E139" s="20">
         <v>1</v>
       </c>
       <c r="F139" s="22">
@@ -5872,15 +5878,15 @@
         <v>0</v>
       </c>
       <c r="H139" s="17" t="s">
-        <v>516</v>
+        <v>288</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="17" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B140" s="23" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C140" s="2">
         <v>0</v>
@@ -5898,15 +5904,15 @@
         <v>0</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="17" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B141" s="23" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C141" s="2">
         <v>0</v>
@@ -5924,15 +5930,15 @@
         <v>0</v>
       </c>
       <c r="H141" s="17" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B142" s="23" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="C142" s="2">
         <v>0</v>
@@ -5950,15 +5956,15 @@
         <v>0</v>
       </c>
       <c r="H142" s="17" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B143" s="23" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="C143" s="2">
         <v>0</v>
@@ -5976,15 +5982,15 @@
         <v>0</v>
       </c>
       <c r="H143" s="17" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C144" s="2">
         <v>0</v>
@@ -6002,15 +6008,15 @@
         <v>0</v>
       </c>
       <c r="H144" s="17" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
@@ -6028,15 +6034,15 @@
         <v>0</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="C146" s="2">
         <v>0</v>
@@ -6054,15 +6060,15 @@
         <v>0</v>
       </c>
       <c r="H146" s="17" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="C147" s="2">
         <v>0</v>
@@ -6080,15 +6086,15 @@
         <v>0</v>
       </c>
       <c r="H147" s="17" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="C148" s="2">
         <v>0</v>
@@ -6106,15 +6112,15 @@
         <v>0</v>
       </c>
       <c r="H148" s="17" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C149" s="2">
         <v>0</v>
@@ -6132,15 +6138,15 @@
         <v>0</v>
       </c>
       <c r="H149" s="17" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C150" s="2">
         <v>0</v>
@@ -6158,15 +6164,15 @@
         <v>0</v>
       </c>
       <c r="H150" s="17" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
@@ -6184,15 +6190,15 @@
         <v>0</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -6210,15 +6216,15 @@
         <v>0</v>
       </c>
       <c r="H152" s="17" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6236,15 +6242,15 @@
         <v>0</v>
       </c>
       <c r="H153" s="17" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
@@ -6262,15 +6268,15 @@
         <v>0</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B155" s="23" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C155" s="2">
         <v>0</v>
@@ -6288,12 +6294,12 @@
         <v>0</v>
       </c>
       <c r="H155" s="17" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B156" s="23" t="s">
         <v>550</v>
@@ -6314,15 +6320,15 @@
         <v>0</v>
       </c>
       <c r="H156" s="17" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
-        <v>452</v>
-      </c>
-      <c r="B157" s="14" t="s">
-        <v>124</v>
+        <v>574</v>
+      </c>
+      <c r="B157" s="23" t="s">
+        <v>549</v>
       </c>
       <c r="C157" s="2">
         <v>0</v>
@@ -6330,7 +6336,7 @@
       <c r="D157" s="2">
         <v>0</v>
       </c>
-      <c r="E157" s="20">
+      <c r="E157" s="4">
         <v>1</v>
       </c>
       <c r="F157" s="22">
@@ -6340,15 +6346,15 @@
         <v>0</v>
       </c>
       <c r="H157" s="17" t="s">
-        <v>289</v>
+        <v>532</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
-        <v>417</v>
+        <v>452</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C158" s="2">
         <v>0</v>
@@ -6366,15 +6372,15 @@
         <v>0</v>
       </c>
       <c r="H158" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
-        <v>453</v>
+        <v>417</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -6389,18 +6395,18 @@
         <v>1</v>
       </c>
       <c r="G159" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H159" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C160" s="2">
         <v>0</v>
@@ -6418,15 +6424,15 @@
         <v>1</v>
       </c>
       <c r="H160" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
-        <v>455</v>
-      </c>
-      <c r="B161" s="15" t="s">
-        <v>128</v>
+        <v>454</v>
+      </c>
+      <c r="B161" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="C161" s="2">
         <v>0</v>
@@ -6441,18 +6447,18 @@
         <v>1</v>
       </c>
       <c r="G161" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H161" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B162" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C162" s="2">
         <v>0</v>
@@ -6470,15 +6476,15 @@
         <v>0</v>
       </c>
       <c r="H162" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
-        <v>457</v>
-      </c>
-      <c r="B163" s="14" t="s">
-        <v>130</v>
+        <v>456</v>
+      </c>
+      <c r="B163" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
@@ -6496,15 +6502,15 @@
         <v>0</v>
       </c>
       <c r="H163" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C164" s="2">
         <v>0</v>
@@ -6515,22 +6521,22 @@
       <c r="E164" s="20">
         <v>1</v>
       </c>
-      <c r="F164" s="20">
+      <c r="F164" s="22">
         <v>1</v>
       </c>
       <c r="G164" s="3">
         <v>0</v>
       </c>
       <c r="H164" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
@@ -6541,22 +6547,22 @@
       <c r="E165" s="20">
         <v>1</v>
       </c>
-      <c r="F165" s="22">
+      <c r="F165" s="20">
         <v>1</v>
       </c>
       <c r="G165" s="3">
         <v>0</v>
       </c>
       <c r="H165" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C166" s="2">
         <v>0</v>
@@ -6574,15 +6580,15 @@
         <v>0</v>
       </c>
       <c r="H166" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B167" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C167" s="2">
         <v>0</v>
@@ -6600,15 +6606,15 @@
         <v>0</v>
       </c>
       <c r="H167" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B168" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C168" s="2">
         <v>0</v>
@@ -6626,15 +6632,15 @@
         <v>0</v>
       </c>
       <c r="H168" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B169" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
@@ -6652,15 +6658,15 @@
         <v>0</v>
       </c>
       <c r="H169" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B170" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -6678,15 +6684,15 @@
         <v>0</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -6704,15 +6710,15 @@
         <v>0</v>
       </c>
       <c r="H171" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -6730,15 +6736,15 @@
         <v>0</v>
       </c>
       <c r="H172" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>588</v>
+        <v>466</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -6756,15 +6762,15 @@
         <v>0</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C174" s="2">
         <v>0</v>
@@ -6782,7 +6788,7 @@
         <v>0</v>
       </c>
       <c r="H174" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -6790,7 +6796,7 @@
         <v>589</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C175" s="2">
         <v>0</v>
@@ -6808,15 +6814,15 @@
         <v>0</v>
       </c>
       <c r="H175" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C176" s="2">
         <v>0</v>
@@ -6834,15 +6840,15 @@
         <v>0</v>
       </c>
       <c r="H176" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
@@ -6860,15 +6866,15 @@
         <v>0</v>
       </c>
       <c r="H177" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="17" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C178" s="2">
         <v>0</v>
@@ -6886,15 +6892,15 @@
         <v>0</v>
       </c>
       <c r="H178" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C179" s="2">
         <v>0</v>
@@ -6912,15 +6918,15 @@
         <v>0</v>
       </c>
       <c r="H179" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C180" s="2">
         <v>0</v>
@@ -6938,15 +6944,15 @@
         <v>0</v>
       </c>
       <c r="H180" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C181" s="2">
         <v>0</v>
@@ -6964,15 +6970,15 @@
         <v>0</v>
       </c>
       <c r="H181" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
@@ -6990,15 +6996,15 @@
         <v>0</v>
       </c>
       <c r="H182" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="17" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C183" s="2">
         <v>0</v>
@@ -7016,15 +7022,15 @@
         <v>0</v>
       </c>
       <c r="H183" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C184" s="2">
         <v>0</v>
@@ -7042,15 +7048,15 @@
         <v>0</v>
       </c>
       <c r="H184" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="17" t="s">
-        <v>467</v>
+        <v>598</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C185" s="2">
         <v>0</v>
@@ -7068,15 +7074,15 @@
         <v>0</v>
       </c>
       <c r="H185" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
@@ -7087,22 +7093,22 @@
       <c r="E186" s="20">
         <v>1</v>
       </c>
-      <c r="F186" s="20">
+      <c r="F186" s="22">
         <v>1</v>
       </c>
       <c r="G186" s="3">
         <v>0</v>
       </c>
       <c r="H186" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -7113,22 +7119,22 @@
       <c r="E187" s="20">
         <v>1</v>
       </c>
-      <c r="F187" s="22">
+      <c r="F187" s="20">
         <v>1</v>
       </c>
       <c r="G187" s="3">
         <v>0</v>
       </c>
       <c r="H187" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -7146,15 +7152,15 @@
         <v>0</v>
       </c>
       <c r="H188" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C189" s="2">
         <v>0</v>
@@ -7172,15 +7178,15 @@
         <v>0</v>
       </c>
       <c r="H189" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7198,15 +7204,15 @@
         <v>0</v>
       </c>
       <c r="H190" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7224,15 +7230,15 @@
         <v>0</v>
       </c>
       <c r="H191" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C192" s="2">
         <v>0</v>
@@ -7250,15 +7256,15 @@
         <v>0</v>
       </c>
       <c r="H192" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C193" s="2">
         <v>0</v>
@@ -7276,15 +7282,15 @@
         <v>0</v>
       </c>
       <c r="H193" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C194" s="2">
         <v>0</v>
@@ -7302,67 +7308,67 @@
         <v>0</v>
       </c>
       <c r="H194" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="17" t="s">
+        <v>476</v>
+      </c>
+      <c r="B195" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C195" s="2">
+        <v>0</v>
+      </c>
+      <c r="D195" s="2">
+        <v>0</v>
+      </c>
+      <c r="E195" s="20">
+        <v>1</v>
+      </c>
+      <c r="F195" s="22">
+        <v>1</v>
+      </c>
+      <c r="G195" s="3">
+        <v>0</v>
+      </c>
+      <c r="H195" s="17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" s="17" t="s">
         <v>477</v>
       </c>
-      <c r="B195" s="14" t="s">
+      <c r="B196" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C195" s="2">
-        <v>0</v>
-      </c>
-      <c r="D195" s="2">
-        <v>0</v>
-      </c>
-      <c r="E195" s="20">
-        <v>1</v>
-      </c>
-      <c r="F195" s="22">
-        <v>1</v>
-      </c>
-      <c r="G195" s="3">
-        <v>0</v>
-      </c>
-      <c r="H195" s="17" t="s">
+      <c r="C196" s="2">
+        <v>0</v>
+      </c>
+      <c r="D196" s="2">
+        <v>0</v>
+      </c>
+      <c r="E196" s="20">
+        <v>1</v>
+      </c>
+      <c r="F196" s="22">
+        <v>1</v>
+      </c>
+      <c r="G196" s="3">
+        <v>0</v>
+      </c>
+      <c r="H196" s="17" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A196" s="18" t="s">
-        <v>478</v>
-      </c>
-      <c r="B196" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C196" s="2">
-        <v>0</v>
-      </c>
-      <c r="D196" s="2">
-        <v>0</v>
-      </c>
-      <c r="E196" s="20">
-        <v>1</v>
-      </c>
-      <c r="F196" s="22">
-        <v>1</v>
-      </c>
-      <c r="G196" s="3">
-        <v>0</v>
-      </c>
-      <c r="H196" s="18" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B197" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C197" s="2">
         <v>0</v>
@@ -7380,15 +7386,15 @@
         <v>0</v>
       </c>
       <c r="H197" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="18" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B198" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C198" s="2">
         <v>0</v>
@@ -7406,15 +7412,15 @@
         <v>0</v>
       </c>
       <c r="H198" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B199" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C199" s="2">
         <v>0</v>
@@ -7432,15 +7438,15 @@
         <v>0</v>
       </c>
       <c r="H199" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="18" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B200" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C200" s="2">
         <v>0</v>
@@ -7458,15 +7464,15 @@
         <v>0</v>
       </c>
       <c r="H200" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B201" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C201" s="2">
         <v>0</v>
@@ -7484,15 +7490,15 @@
         <v>0</v>
       </c>
       <c r="H201" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="18" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B202" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C202" s="2">
         <v>0</v>
@@ -7510,32 +7516,58 @@
         <v>0</v>
       </c>
       <c r="H202" s="18" t="s">
-        <v>214</v>
+        <v>333</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="B203" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C203" s="2">
+        <v>0</v>
+      </c>
+      <c r="D203" s="2">
+        <v>0</v>
+      </c>
+      <c r="E203" s="20">
+        <v>1</v>
+      </c>
+      <c r="F203" s="22">
+        <v>1</v>
+      </c>
+      <c r="G203" s="3">
+        <v>0</v>
+      </c>
+      <c r="H203" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" s="18" t="s">
         <v>485</v>
       </c>
-      <c r="B203" s="16" t="s">
+      <c r="B204" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C203" s="2">
-        <v>0</v>
-      </c>
-      <c r="D203" s="2">
-        <v>0</v>
-      </c>
-      <c r="E203" s="20">
-        <v>1</v>
-      </c>
-      <c r="F203" s="20">
-        <v>1</v>
-      </c>
-      <c r="G203" s="3">
-        <v>0</v>
-      </c>
-      <c r="H203" s="18" t="s">
+      <c r="C204" s="2">
+        <v>0</v>
+      </c>
+      <c r="D204" s="2">
+        <v>0</v>
+      </c>
+      <c r="E204" s="20">
+        <v>1</v>
+      </c>
+      <c r="F204" s="20">
+        <v>1</v>
+      </c>
+      <c r="G204" s="3">
+        <v>0</v>
+      </c>
+      <c r="H204" s="18" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update hospitalisation follow-up logs to look for lost-to-follow-up referred children
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_senegal.xlsx
+++ b/inst/extdata/main_dict_senegal.xlsx
@@ -2030,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>